<commit_message>
Update pembayaran: tambah data pengiriman & perbaikan struktur riwayat
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/riwayat_pembayaran.xlsx
+++ b/DASHBOARD_main/riwayat_pembayaran.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,290 +464,74 @@
           <t>Metode</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Nama_Penerima</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>No_HP</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Alamat</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Jasa_Pengiriman</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2345678990112444</t>
+          <t>9801234567819235</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BG6701HI</t>
+          <t>BG8799BI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tiara</t>
+          <t>Dinda</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>01-08-2025 05:09</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>10000</t>
-        </is>
+          <t>01-08-2025 23:19</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>10000</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BRI</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2345678990112444</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BG6701HI</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Tiara</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>01-08-2025 05:15</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>BRI</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2345678990112444</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>BG6701HI</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Tiara</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>01-08-2025 05:16</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>BRI</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2345678990112444</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>BG6701HI</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Tiara</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>01-08-2025 05:24</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>BRI</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2345678990112444</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>BG6701HI</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Tiara</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>01-08-2025 05:35</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>BRI</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2345678990112444</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>BG6701HI</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Tiara</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>01-08-2025 06:23</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
           <t>Bank Rakyat Indonesia (BRI)</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1234456278949542</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>BG4576HI</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Nia</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>01-08-2025 06:28</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Bank Syariah Indonesia (BSI)</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1234456278949542</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>BG4576HI</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Nia</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>01-08-2025 06:28</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>20000</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Bank Mandiri</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9801234567819235</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>BG8799BI</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Dinda</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>01-08-2025 08:37</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Bank Mandiri</t>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>089012736819h</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Jl. Melati, Palembang</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>JNE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix format tanggal dan visualisasi tren pembayaran
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/riwayat_pembayaran.xlsx
+++ b/DASHBOARD_main/riwayat_pembayaran.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -870,8 +870,10 @@
           <t>02-08-2025 17:59</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>65000</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -896,6 +898,680 @@
       <c r="J9" t="inlineStr">
         <is>
           <t>J&amp;T</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>05-08-2025 03:16</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>GoPay</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>05-08-2025 03:46</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Bank Mandiri</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>05-08-2025 03:52</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Bank Mandiri</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>05-08-2025 04:04</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Bank Mandiri</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>05-08-2025 04:05</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Bank Mandiri</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>05-08-2025 04:07</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>SeaBank</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>05-08-2025 04:09</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>SeaBank</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>05-08-2025 04:10</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>SeaBank</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>05-08-2025 11:16</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>SeaBank</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>05-08-2025 11:17</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Bank Rakyat Indonesia (BRI)</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>08-05-2025 11:41</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Bank Central Asia (BCA)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>05-08-2025 11:46</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Bank Rakyat Indonesia (BRI)</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>JNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>1234456278949542</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BG4576HI</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>05-08-2025 11:50</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>30000</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Bank Rakyat Indonesia (BRI)</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nia Rahmadani</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>085267947261</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>JNE</t>
         </is>
       </c>
     </row>

</xml_diff>